<commit_message>
Update New Bulk User Upload Template to reflect new data structure
</commit_message>
<xml_diff>
--- a/public/NewBulkUserUploadTemplate.xlsx
+++ b/public/NewBulkUserUploadTemplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Full Name</t>
   </si>
@@ -42,114 +42,6 @@
   </si>
   <si>
     <t>Department</t>
-  </si>
-  <si>
-    <t>Aklilu Haile Abitew</t>
-  </si>
-  <si>
-    <t>akilshm9631@gmail.com</t>
-  </si>
-  <si>
-    <t>here</t>
-  </si>
-  <si>
-    <t>there</t>
-  </si>
-  <si>
-    <t>Asregdew Mesele Shibeshi</t>
-  </si>
-  <si>
-    <t>asregedewm@gmail.com</t>
-  </si>
-  <si>
-    <t>Balcha Debebe Tadesse</t>
-  </si>
-  <si>
-    <t>balcha.ta@gmail.com</t>
-  </si>
-  <si>
-    <t>Bezialem Sintayehu Gebru</t>
-  </si>
-  <si>
-    <t>bezihalem24@gmail.com</t>
-  </si>
-  <si>
-    <t>Biniyam Mersha Haile</t>
-  </si>
-  <si>
-    <t>biniammer@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel Walellgn </t>
-  </si>
-  <si>
-    <t>walellgndaniel@gmail.com</t>
-  </si>
-  <si>
-    <t>Endale Shiferaw Worku</t>
-  </si>
-  <si>
-    <t>endaleshiferaw270@gmail.com</t>
-  </si>
-  <si>
-    <t>Girum Zena Tegegn</t>
-  </si>
-  <si>
-    <t>girumzena@gmail.com</t>
-  </si>
-  <si>
-    <t>Merid Kebede Weldeyes</t>
-  </si>
-  <si>
-    <t>kebedemerid212@gmail.com</t>
-  </si>
-  <si>
-    <t>Muche Ambisa Yadesa</t>
-  </si>
-  <si>
-    <t>mucheastu7@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nigussie Kebede </t>
-  </si>
-  <si>
-    <t>negussiekebede06@gmail.com</t>
-  </si>
-  <si>
-    <t>Sori Milkesa Gonfa</t>
-  </si>
-  <si>
-    <t>milkesasor877@gmail.com</t>
-  </si>
-  <si>
-    <t>Tesfaye Borcha Bololo</t>
-  </si>
-  <si>
-    <t>tesfayeboricha7@gmail.com</t>
-  </si>
-  <si>
-    <t>Yoseph Birhanu Tassew</t>
-  </si>
-  <si>
-    <t>yosephrich123@gmail.com</t>
-  </si>
-  <si>
-    <t>Sileshi Demisse Borena</t>
-  </si>
-  <si>
-    <t>sileshidemissie.41@gmail.com</t>
-  </si>
-  <si>
-    <t>Bereket Bogale</t>
-  </si>
-  <si>
-    <t>bekayaeng@gmail.com</t>
-  </si>
-  <si>
-    <t>Sr. Telelech Befikadu</t>
-  </si>
-  <si>
-    <t>teleb@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1155,16 +1047,16 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="27.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="22.4444444444444" customWidth="1"/>
-    <col min="3" max="3" width="14.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="27.775" customWidth="1"/>
+    <col min="2" max="2" width="22.4416666666667" customWidth="1"/>
+    <col min="3" max="3" width="14.1083333333333" customWidth="1"/>
     <col min="4" max="4" width="9.66666666666667" customWidth="1"/>
-    <col min="5" max="5" width="11.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="11.8916666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1184,315 +1076,75 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>2519478597</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" ht="15.6" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>2519478598</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" ht="15.6" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>2519478599</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" ht="15.6" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>2519478600</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" ht="15.6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>2519478601</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" ht="15.6" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>2519478602</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" ht="15.6" spans="1:5">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>2519478603</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" ht="15.6" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9">
-        <v>2519478604</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" ht="15.6" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
-        <v>2519478605</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" ht="15.6" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>2519478606</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" ht="15.6" spans="1:5">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>2519478607</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" ht="15.6" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13">
-        <v>2519478608</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" ht="15.6" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14">
-        <v>2519478609</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" ht="15.6" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15">
-        <v>2519478610</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" ht="15.6" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16">
-        <v>2519478611</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" ht="15.6" spans="1:5">
-      <c r="A17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17">
-        <v>2519478612</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" ht="15.6" spans="1:5">
-      <c r="A18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18">
-        <v>2519478613</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
+    <row r="2" ht="15.6" spans="1:2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" ht="15.6" spans="1:2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" ht="15.6" spans="1:2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" ht="15.6" spans="1:2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" ht="15.6" spans="1:2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" ht="15.6" spans="1:2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" ht="15.6" spans="1:2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" ht="15.6" spans="1:2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" ht="15.6" spans="1:2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" ht="15.6" spans="1:2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" ht="15.6" spans="1:2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" ht="15.6" spans="1:2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" ht="15.6" spans="1:2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" ht="15.6" spans="1:2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" ht="15.6" spans="1:2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" ht="15.6" spans="1:2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" ht="15.6" spans="1:2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="biniammer@gmail.com"/>
-    <hyperlink ref="B17" r:id="rId2" display="bekayaeng@gmail.com"/>
-    <hyperlink ref="B12" r:id="rId3" display="negussiekebede06@gmail.com"/>
-    <hyperlink ref="B15" r:id="rId4" display="yosephrich123@gmail.com"/>
-    <hyperlink ref="B13" r:id="rId5" display="milkesasor877@gmail.com"/>
-    <hyperlink ref="B14" r:id="rId6" display="tesfayeboricha7@gmail.com"/>
-    <hyperlink ref="B10" r:id="rId7" display="kebedemerid212@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId8" display="asregedewm@gmail.com"/>
-    <hyperlink ref="B11" r:id="rId9" display="mucheastu7@gmail.com"/>
-    <hyperlink ref="B16" r:id="rId10" display="sileshidemissie.41@gmail.com"/>
-    <hyperlink ref="B7" r:id="rId11" display="walellgndaniel@gmail.com"/>
-    <hyperlink ref="B5" r:id="rId12" display="bezihalem24@gmail.com"/>
-    <hyperlink ref="B9" r:id="rId13" display="girumzena@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId14" display="akilshm9631@gmail.com"/>
-    <hyperlink ref="B4" r:id="rId15" display="balcha.ta@gmail.com"/>
-    <hyperlink ref="B8" r:id="rId16" display="endaleshiferaw270@gmail.com"/>
-    <hyperlink ref="B18" r:id="rId17" display="teleb@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>

</xml_diff>